<commit_message>
Actualizacion página con listado de locales
</commit_message>
<xml_diff>
--- a/Excel Locales/LOCALES Y RUBROS V3.xlsx
+++ b/Excel Locales/LOCALES Y RUBROS V3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="96" windowWidth="19980" windowHeight="7308"/>
+    <workbookView xWindow="240" yWindow="96" windowWidth="19980" windowHeight="7308" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="182">
   <si>
     <t>LOCALES</t>
   </si>
@@ -723,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -744,39 +744,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1081,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,26 +1099,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="16" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="24" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26" t="s">
         <v>147</v>
       </c>
       <c r="M1" s="15"/>
@@ -1263,10 +1264,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="19" t="s">
         <v>17</v>
       </c>
@@ -1833,12 +1834,12 @@
         <v>70</v>
       </c>
       <c r="D31" s="19"/>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="4" t="s">
         <v>137</v>
       </c>
@@ -2000,12 +2001,12 @@
         <v>85</v>
       </c>
       <c r="D38" s="19"/>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
       <c r="I38" s="4" t="s">
         <v>143</v>
       </c>
@@ -2026,12 +2027,12 @@
         <v>88</v>
       </c>
       <c r="D39" s="19"/>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="4" t="s">
         <v>144</v>
       </c>
@@ -2040,20 +2041,20 @@
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="22" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
       <c r="I40" s="4" t="s">
         <v>145</v>
       </c>
@@ -2062,20 +2063,20 @@
       <c r="M40" s="9"/>
     </row>
     <row r="41" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="20" t="s">
+      <c r="B41" s="18"/>
+      <c r="C41" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="20" t="s">
+      <c r="D41" s="18"/>
+      <c r="E41" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="4" t="s">
         <v>146</v>
       </c>
@@ -2091,17 +2092,17 @@
       <c r="M42" s="9"/>
     </row>
     <row r="43" spans="1:16" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
@@ -2145,6 +2146,113 @@
     </row>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
@@ -2169,113 +2277,6 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
@@ -2314,13 +2315,529 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <f>LOWER(B2)</f>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f t="shared" ref="C3:C41" si="0">LOWER(B3)</f>
+        <v>infantiles (regaleria y productos para niños)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria unisex</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>joyeria y bijouteri (marrouqineria, bijouteri y accesorios)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>lenceria</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria infantil</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria masculina</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria unisex (deportiva)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria infantil</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria masculina</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>otros (merceria, arreglos y afines)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria masculina</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina (ropa de fiesta)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>marroquineria y calzados</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>tecnologia y entretenimiento (librería)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>lenceria</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>gastronomia (pizzeria)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>infantiles (cotillon)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria infantil</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>gastronomia (pasteleria)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>joyeria y bijouterie (joyeria y relojeria)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>joyeria y bijouteria (joyeria y relojeria)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>supermercado (productos alimenticos, y varios)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>marroquineria y calzados</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>infantiles (jugeteria)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>cuidados personales (perfumeria)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina (corregir, en la pagina esta en joyeria y bijouteri)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>otros (cortinas, toldos y accesorios)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria masculina</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>gastronomia (bar y cafeteria)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>indumentaria femenina</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>tecnologia y entretenimiento</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>gastronomia (bomboneria)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>marroquineria y calzados</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B41">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Agregado de paginas de rubros.
</commit_message>
<xml_diff>
--- a/Excel Locales/LOCALES Y RUBROS V3.xlsx
+++ b/Excel Locales/LOCALES Y RUBROS V3.xlsx
@@ -741,19 +741,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -762,22 +772,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1099,29 +1099,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="M1" s="15"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="13" t="s">
         <v>167</v>
       </c>
@@ -1132,20 +1132,20 @@
       <c r="Q1" s="14"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="2" t="s">
         <v>111</v>
       </c>
@@ -1159,20 +1159,20 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="2" t="s">
         <v>112</v>
       </c>
@@ -1181,20 +1181,20 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="2" t="s">
         <v>113</v>
       </c>
@@ -1208,20 +1208,20 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="4" t="s">
         <v>114</v>
       </c>
@@ -1238,20 +1238,20 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="4" t="s">
         <v>115</v>
       </c>
@@ -1260,20 +1260,20 @@
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="4" t="s">
         <v>116</v>
       </c>
@@ -1284,20 +1284,20 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
       <c r="I8" s="4" t="s">
         <v>117</v>
       </c>
@@ -1308,20 +1308,20 @@
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="3" t="s">
         <v>118</v>
       </c>
@@ -1332,20 +1332,20 @@
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="5" t="s">
         <v>119</v>
       </c>
@@ -1359,20 +1359,20 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
       <c r="I11" s="5" t="s">
         <v>120</v>
       </c>
@@ -1384,20 +1384,20 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="5" t="s">
         <v>121</v>
       </c>
@@ -1406,20 +1406,20 @@
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="5" t="s">
         <v>122</v>
       </c>
@@ -1434,20 +1434,20 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="5" t="s">
         <v>123</v>
       </c>
@@ -1456,20 +1456,20 @@
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="5" t="s">
         <v>124</v>
       </c>
@@ -1478,40 +1478,40 @@
       <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="5" t="s">
         <v>125</v>
       </c>
@@ -1522,20 +1522,20 @@
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="L18" s="10" t="s">
@@ -1544,20 +1544,20 @@
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="5" t="s">
         <v>126</v>
       </c>
@@ -1568,20 +1568,20 @@
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="5" t="s">
         <v>127</v>
       </c>
@@ -1592,20 +1592,20 @@
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="5" t="s">
         <v>128</v>
       </c>
@@ -1617,20 +1617,20 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="5" t="s">
         <v>129</v>
       </c>
@@ -1641,20 +1641,20 @@
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="5" t="s">
         <v>130</v>
       </c>
@@ -1663,20 +1663,20 @@
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="5" t="s">
         <v>131</v>
       </c>
@@ -1687,20 +1687,20 @@
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="5" t="s">
         <v>132</v>
       </c>
@@ -1709,20 +1709,20 @@
       <c r="M25" s="9"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="5" t="s">
         <v>133</v>
       </c>
@@ -1736,20 +1736,20 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="s">
+      <c r="D27" s="16"/>
+      <c r="E27" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="5" t="s">
         <v>134</v>
       </c>
@@ -1760,20 +1760,20 @@
       <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="5" t="s">
         <v>135</v>
       </c>
@@ -1784,40 +1784,40 @@
       <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="I30" s="5" t="s">
         <v>136</v>
       </c>
@@ -1826,15 +1826,15 @@
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="21" t="s">
         <v>148</v>
       </c>
       <c r="F31" s="22"/>
@@ -1850,20 +1850,20 @@
       <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19" t="s">
+      <c r="D32" s="16"/>
+      <c r="E32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
       <c r="I32" s="4" t="s">
         <v>138</v>
       </c>
@@ -1874,20 +1874,20 @@
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33" s="4" t="s">
         <v>135</v>
       </c>
@@ -1898,20 +1898,20 @@
       <c r="M33" s="9"/>
     </row>
     <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34" s="4" t="s">
         <v>139</v>
       </c>
@@ -1922,20 +1922,20 @@
       <c r="M34" s="12"/>
     </row>
     <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="I35" s="4" t="s">
         <v>140</v>
       </c>
@@ -1946,14 +1946,14 @@
       <c r="M35" s="9"/>
     </row>
     <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="6" t="s">
         <v>81</v>
       </c>
@@ -1971,20 +1971,20 @@
       <c r="M36" s="9"/>
     </row>
     <row r="37" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="I37" s="4" t="s">
         <v>142</v>
       </c>
@@ -1993,41 +1993,41 @@
       <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19" t="s">
+      <c r="B38" s="16"/>
+      <c r="C38" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="4" t="s">
         <v>143</v>
       </c>
       <c r="J38" s="3"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
-      <c r="O38" s="15" t="s">
+      <c r="O38" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="P38" s="15"/>
+      <c r="P38" s="17"/>
     </row>
     <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="17" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="21" t="s">
         <v>97</v>
       </c>
       <c r="F39" s="22"/>
@@ -2041,20 +2041,20 @@
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20" t="s">
+      <c r="B40" s="24"/>
+      <c r="C40" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
+      <c r="D40" s="24"/>
+      <c r="E40" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
       <c r="I40" s="4" t="s">
         <v>145</v>
       </c>
@@ -2063,15 +2063,15 @@
       <c r="M40" s="9"/>
     </row>
     <row r="41" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="17" t="s">
+      <c r="B41" s="27"/>
+      <c r="C41" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="17" t="s">
+      <c r="D41" s="27"/>
+      <c r="E41" s="21" t="s">
         <v>102</v>
       </c>
       <c r="F41" s="22"/>
@@ -2092,17 +2092,17 @@
       <c r="M42" s="9"/>
     </row>
     <row r="43" spans="1:16" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
@@ -2111,41 +2111,148 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="15"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="15"/>
+      <c r="B46" s="17"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="15"/>
+      <c r="B47" s="17"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="15"/>
+      <c r="B48" s="17"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="15"/>
+      <c r="B49" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="131">
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="O38:P38"/>
     <mergeCell ref="I1:K1"/>
@@ -2170,113 +2277,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C40:D40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
@@ -2317,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2329,13 +2329,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">

</xml_diff>